<commit_message>
small fix to put excel
</commit_message>
<xml_diff>
--- a/Projects/Transgender/results.xlsx
+++ b/Projects/Transgender/results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4152" uniqueCount="171">
   <si>
     <t>new_sssi_e</t>
   </si>
@@ -491,6 +491,45 @@
   </si>
   <si>
     <t>19 (6.13%)</t>
+  </si>
+  <si>
+    <t>6 (1.52%)</t>
+  </si>
+  <si>
+    <t>1 (0.25%)</t>
+  </si>
+  <si>
+    <t>7 (1.77%)</t>
+  </si>
+  <si>
+    <t>2 (0.97%)</t>
+  </si>
+  <si>
+    <t>6 (2.91%)</t>
+  </si>
+  <si>
+    <t>7 (3.40%)</t>
+  </si>
+  <si>
+    <t>1 (3.23%)</t>
+  </si>
+  <si>
+    <t>1 (0.71%)</t>
+  </si>
+  <si>
+    <t>14 (10.00%)</t>
+  </si>
+  <si>
+    <t>4 (2.86%)</t>
+  </si>
+  <si>
+    <t>19 (13.57%)</t>
+  </si>
+  <si>
+    <t>Outcome does not vary</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -565,22 +604,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>161</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>165</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -597,13 +636,13 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>166</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -657,22 +696,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>162</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>167</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -749,22 +788,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just before abstracting out encode_and_label_binary
</commit_message>
<xml_diff>
--- a/Projects/Transgender/results.xlsx
+++ b/Projects/Transgender/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2463" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5208" uniqueCount="286">
   <si>
     <t>Variable</t>
   </si>
@@ -523,6 +523,357 @@
   </si>
   <si>
     <t>Diabetes</t>
+  </si>
+  <si>
+    <t>OR_Any_Complication</t>
+  </si>
+  <si>
+    <t>FTM Top Surgery</t>
+  </si>
+  <si>
+    <t>0.35 (0.15-0.81)</t>
+  </si>
+  <si>
+    <t>Hysterectomy/Oophorectomy</t>
+  </si>
+  <si>
+    <t>0.92 (0.40-2.15)</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>Vaginectomy/Vulvectomy</t>
+  </si>
+  <si>
+    <t>0.89 (0.12-6.70)</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>MTF Top Surgery</t>
+  </si>
+  <si>
+    <t>MTF Bottom Surgery</t>
+  </si>
+  <si>
+    <t>8.24 (4.08-16.65)</t>
+  </si>
+  <si>
+    <t>Head/Neck Surgery</t>
+  </si>
+  <si>
+    <t>Race: American Indian or Alaska Native</t>
+  </si>
+  <si>
+    <t>7 (0.96%)</t>
+  </si>
+  <si>
+    <t>3 (0.63%)</t>
+  </si>
+  <si>
+    <t>4 (1.59%)</t>
+  </si>
+  <si>
+    <t>Race: Asian</t>
+  </si>
+  <si>
+    <t>25 (5.23%)</t>
+  </si>
+  <si>
+    <t>12 (4.78%)</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>Race: Black of African American</t>
+  </si>
+  <si>
+    <t>90 (12.35%)</t>
+  </si>
+  <si>
+    <t>45 (9.41%)</t>
+  </si>
+  <si>
+    <t>45 (17.93%)</t>
+  </si>
+  <si>
+    <t>Native Hawaiian or Pacific Islander</t>
+  </si>
+  <si>
+    <t>2 (0.27%)</t>
+  </si>
+  <si>
+    <t>1 (0.21%)</t>
+  </si>
+  <si>
+    <t>1 (0.40%)</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>593 (81.34%)</t>
+  </si>
+  <si>
+    <t>404 (84.52%)</t>
+  </si>
+  <si>
+    <t>189 (75.30%)</t>
+  </si>
+  <si>
+    <t>Previous Sepsis</t>
+  </si>
+  <si>
+    <t>1 (0.11%)</t>
+  </si>
+  <si>
+    <t>1 (0.16%)</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>New Deep Surgical Site Infection</t>
+  </si>
+  <si>
+    <t>2 (0.21%)</t>
+  </si>
+  <si>
+    <t>2 (0.65%)</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>New Organ Space Infection</t>
+  </si>
+  <si>
+    <t>3 (0.47%)</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>Stroke/CVA with neurological deficit</t>
+  </si>
+  <si>
+    <t>Pulmonary Embolism</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>37 (3.93%)</t>
+  </si>
+  <si>
+    <t>18 (2.85%)</t>
+  </si>
+  <si>
+    <t>9 (4.37%)</t>
+  </si>
+  <si>
+    <t>2 (6.45%)</t>
+  </si>
+  <si>
+    <t>2 (1.43%)</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>1.08 (0.73-1.61)</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.81 (0.33-1.98)</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>2.41 (0.54-10.66)</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>1.99 (0.75-5.27)</t>
+  </si>
+  <si>
+    <t>0.17</t>
+  </si>
+  <si>
+    <t>1.68 (0.64-4.44)</t>
+  </si>
+  <si>
+    <t>0.29</t>
+  </si>
+  <si>
+    <t>1.17 (0.59-2.33)</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>1.14 (0.53-2.46)</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>0.82 (0.19-3.49)</t>
+  </si>
+  <si>
+    <t>2.23 (1.15-4.31)</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>0.16 (0.07-0.36)</t>
+  </si>
+  <si>
+    <t>0.31 (0.14-0.72)</t>
+  </si>
+  <si>
+    <t>1.16 (0.54-2.49)</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>1.73 (0.40-7.52)</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>6.84 (3.49-13.40)</t>
+  </si>
+  <si>
+    <t>History of TIA/CVA</t>
+  </si>
+  <si>
+    <t>History of Cardiac Ischemia</t>
+  </si>
+  <si>
+    <t>History of PVD, rest pain or gangrene</t>
+  </si>
+  <si>
+    <t>Bleeding Transfusions</t>
+  </si>
+  <si>
+    <t>5 (0.53%)</t>
+  </si>
+  <si>
+    <t>Systemic Sepsis or Septic Schock</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>MI, Cardiac Arrest or CVA</t>
+  </si>
+  <si>
+    <t>Reintubation or Failure to Wean Vent</t>
+  </si>
+  <si>
+    <t>43 (4.56%)</t>
+  </si>
+  <si>
+    <t>22 (3.48%)</t>
+  </si>
+  <si>
+    <t>21 (6.77%)</t>
+  </si>
+  <si>
+    <t>8 (2.03%)</t>
+  </si>
+  <si>
+    <t>1 (0.49%)</t>
+  </si>
+  <si>
+    <t>10 (4.85%)</t>
+  </si>
+  <si>
+    <t>4 (12.90%)</t>
+  </si>
+  <si>
+    <t>21 (15.00%)</t>
+  </si>
+  <si>
+    <t>0.19</t>
+  </si>
+  <si>
+    <t>0.94 (0.68-1.30)</t>
+  </si>
+  <si>
+    <t>0.97 (0.44-2.12)</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>2.04 (0.46-8.99)</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>2.08 (0.85-5.11)</t>
+  </si>
+  <si>
+    <t>0.11</t>
+  </si>
+  <si>
+    <t>1.76 (0.72-4.29)</t>
+  </si>
+  <si>
+    <t>1.07 (0.57-2.01)</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>1.07 (0.52-2.21)</t>
+  </si>
+  <si>
+    <t>1.09 (0.33-3.62)</t>
+  </si>
+  <si>
+    <t>2.01 (1.09-3.72)</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.15 (0.07-0.33)</t>
+  </si>
+  <si>
+    <t>0.30 (0.14-0.66)</t>
+  </si>
+  <si>
+    <t>1.09 (0.53-2.24)</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>3.31 (1.10-9.93)</t>
+  </si>
+  <si>
+    <t>6.26 (3.34-11.73)</t>
   </si>
 </sst>
 </file>
@@ -566,7 +917,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F24"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -651,127 +1002,127 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="B5">
         <v>729</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="B6">
-        <v>942</v>
+        <v>729</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>187</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>188</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="B7">
-        <v>942</v>
+        <v>729</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>192</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="B8">
-        <v>942</v>
+        <v>729</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>195</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>199</v>
       </c>
       <c r="B9">
-        <v>942</v>
+        <v>729</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10">
         <v>942</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B11">
         <v>942</v>
@@ -791,121 +1142,261 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="B12">
         <v>942</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>941</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>204</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>205</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B14">
         <v>942</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B15">
         <v>942</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B16">
-        <v>23</v>
+        <v>942</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17">
+        <v>942</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18">
+        <v>942</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19">
+        <v>942</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20">
+        <v>942</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21">
+        <v>942</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22">
+        <v>942</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
         <v>151</v>
       </c>
-      <c r="B17">
-        <v>942</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B24">
+        <v>942</v>
+      </c>
+      <c r="C24" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D24" t="s">
         <v>71</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E24" t="s">
         <v>72</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F24" t="s">
         <v>29</v>
       </c>
     </row>
@@ -915,7 +1406,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F20"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -960,87 +1451,87 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>207</v>
       </c>
       <c r="B3">
         <v>942</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>208</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="B4">
         <v>942</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>212</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>942</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>942</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>942</v>
@@ -1060,27 +1551,27 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8">
-        <v>102</v>
+        <v>942</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9">
         <v>942</v>
@@ -1100,22 +1591,222 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10">
+        <v>942</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12">
+        <v>942</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13">
+        <v>942</v>
+      </c>
+      <c r="C13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15">
+        <v>942</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16">
+        <v>942</v>
+      </c>
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17">
+        <v>942</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18">
+        <v>942</v>
+      </c>
+      <c r="C18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19">
+        <v>942</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>160</v>
       </c>
-      <c r="B10">
-        <v>942</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
+      <c r="B20">
+        <v>942</v>
+      </c>
+      <c r="C20" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" t="s">
+        <v>258</v>
+      </c>
+      <c r="E20" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1124,7 +1815,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C30"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1132,6 +1823,9 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1143,7 +1837,7 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3">
@@ -1154,67 +1848,67 @@
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>269</v>
       </c>
       <c r="C7" t="s">
-        <v>115</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
         <v>114</v>
@@ -1225,7 +1919,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
         <v>114</v>
@@ -1236,7 +1930,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
         <v>114</v>
@@ -1247,7 +1941,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
         <v>114</v>
@@ -1258,51 +1952,51 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>271</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="B14" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>274</v>
       </c>
       <c r="C15" t="s">
-        <v>122</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B17" t="s">
         <v>114</v>
@@ -1313,40 +2007,40 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>276</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>277</v>
       </c>
       <c r="C19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B21" t="s">
         <v>114</v>
@@ -1357,35 +2051,101 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>114</v>
+        <v>278</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>151</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>280</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>281</v>
       </c>
       <c r="C24" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" t="s">
+        <v>282</v>
+      </c>
+      <c r="C25" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" t="s">
+        <v>284</v>
+      </c>
+      <c r="C26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>178</v>
+      </c>
+      <c r="B27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B28" t="s">
+        <v>285</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" t="s">
+        <v>273</v>
+      </c>
+      <c r="C30" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1394,7 +2154,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1445,7 +2205,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -1460,7 +2220,7 @@
         <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>221</v>
       </c>
       <c r="G3" t="s">
         <v>63</v>
@@ -1468,76 +2228,76 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
@@ -1560,30 +2320,30 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
@@ -1606,24 +2366,254 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>221</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>256</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>216</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
         <v>160</v>
       </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="B20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C20" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" t="s">
+        <v>263</v>
+      </c>
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>264</v>
+      </c>
+      <c r="G20" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reversed dependent and independent in put_in_excel file
</commit_message>
<xml_diff>
--- a/Projects/Transgender/results.xlsx
+++ b/Projects/Transgender/results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7320" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8138" uniqueCount="473">
   <si>
     <t>Observations</t>
   </si>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>439</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>438</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>17</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>439</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>438</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -1847,13 +1847,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>438</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>27</v>
@@ -1867,13 +1867,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>439</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>438</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>33</v>
@@ -1887,13 +1887,13 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>439</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>438</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -1907,13 +1907,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>439</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>438</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>439</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>438</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
         <v>50</v>
@@ -1947,13 +1947,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>438</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
         <v>56</v>
@@ -1967,13 +1967,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>439</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>438</v>
+        <v>61</v>
       </c>
       <c r="D10" t="s">
         <v>62</v>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>439</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>438</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
         <v>68</v>
@@ -2007,13 +2007,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>439</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>438</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
         <v>73</v>
@@ -2027,13 +2027,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>439</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>438</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
         <v>79</v>
@@ -2047,13 +2047,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>439</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>82</v>
       </c>
       <c r="C14" t="s">
-        <v>438</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
         <v>84</v>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>438</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
         <v>89</v>
@@ -2087,13 +2087,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>439</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>438</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
         <v>95</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>98</v>
       </c>
       <c r="B17">
         <v>739</v>
@@ -2127,7 +2127,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>439</v>
+        <v>103</v>
       </c>
       <c r="B18">
         <v>739</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>439</v>
+        <v>108</v>
       </c>
       <c r="B19">
         <v>739</v>
@@ -2167,7 +2167,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>439</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>739</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>439</v>
+        <v>117</v>
       </c>
       <c r="B21">
         <v>739</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>122</v>
       </c>
       <c r="B22">
         <v>953</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>439</v>
+        <v>127</v>
       </c>
       <c r="B23">
         <v>953</v>
@@ -2247,7 +2247,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>439</v>
+        <v>130</v>
       </c>
       <c r="B24">
         <v>953</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>439</v>
+        <v>135</v>
       </c>
       <c r="B25">
         <v>952</v>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>439</v>
+        <v>140</v>
       </c>
       <c r="B26">
         <v>953</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>439</v>
+        <v>141</v>
       </c>
       <c r="B27">
         <v>953</v>
@@ -2327,7 +2327,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>439</v>
+        <v>146</v>
       </c>
       <c r="B28">
         <v>953</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>439</v>
+        <v>147</v>
       </c>
       <c r="B29">
         <v>953</v>
@@ -2367,7 +2367,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>439</v>
+        <v>148</v>
       </c>
       <c r="B30">
         <v>953</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>439</v>
+        <v>153</v>
       </c>
       <c r="B31">
         <v>953</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>439</v>
+        <v>158</v>
       </c>
       <c r="B32">
         <v>953</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>439</v>
+        <v>159</v>
       </c>
       <c r="B33">
         <v>953</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>439</v>
+        <v>160</v>
       </c>
       <c r="B34">
         <v>953</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>439</v>
+        <v>161</v>
       </c>
       <c r="B35">
         <v>953</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>439</v>
+        <v>165</v>
       </c>
       <c r="B36">
         <v>953</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>439</v>
+        <v>166</v>
       </c>
       <c r="B37">
         <v>953</v>
@@ -2527,7 +2527,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>439</v>
+        <v>170</v>
       </c>
       <c r="B38">
         <v>953</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>439</v>
+        <v>173</v>
       </c>
       <c r="B39">
         <v>953</v>
@@ -2567,7 +2567,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>439</v>
+        <v>176</v>
       </c>
       <c r="B40">
         <v>953</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>439</v>
+        <v>179</v>
       </c>
       <c r="B41">
         <v>23</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>439</v>
+        <v>184</v>
       </c>
       <c r="B42">
         <v>953</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>439</v>
+        <v>3</v>
       </c>
       <c r="B43">
         <v>953</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>439</v>
+        <v>190</v>
       </c>
       <c r="B44">
         <v>953</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>439</v>
+        <v>192</v>
       </c>
       <c r="B45">
         <v>953</v>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>439</v>
+        <v>195</v>
       </c>
       <c r="B46">
         <v>953</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>439</v>
+        <v>197</v>
       </c>
       <c r="B47">
         <v>953</v>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>439</v>
+        <v>199</v>
       </c>
       <c r="B48">
         <v>953</v>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>439</v>
+        <v>202</v>
       </c>
       <c r="B49">
         <v>953</v>
@@ -2767,7 +2767,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B50">
         <v>953</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>439</v>
+        <v>208</v>
       </c>
       <c r="B51">
         <v>953</v>
@@ -2807,7 +2807,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>439</v>
+        <v>211</v>
       </c>
       <c r="B52">
         <v>953</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>439</v>
+        <v>212</v>
       </c>
       <c r="B53">
         <v>953</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>439</v>
+        <v>216</v>
       </c>
       <c r="B54">
         <v>953</v>
@@ -2900,7 +2900,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>439</v>
+        <v>220</v>
       </c>
       <c r="B2">
         <v>953</v>
@@ -2920,7 +2920,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>439</v>
+        <v>224</v>
       </c>
       <c r="B3">
         <v>953</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>227</v>
       </c>
       <c r="B4">
         <v>953</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>439</v>
+        <v>230</v>
       </c>
       <c r="B5">
         <v>953</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>439</v>
+        <v>231</v>
       </c>
       <c r="B6">
         <v>953</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>439</v>
+        <v>232</v>
       </c>
       <c r="B7">
         <v>953</v>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>439</v>
+        <v>233</v>
       </c>
       <c r="B8">
         <v>953</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>439</v>
+        <v>234</v>
       </c>
       <c r="B9">
         <v>953</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>439</v>
+        <v>235</v>
       </c>
       <c r="B10">
         <v>953</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>439</v>
+        <v>237</v>
       </c>
       <c r="B11">
         <v>953</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>439</v>
+        <v>238</v>
       </c>
       <c r="B12">
         <v>953</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>439</v>
+        <v>240</v>
       </c>
       <c r="B13">
         <v>953</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>439</v>
+        <v>241</v>
       </c>
       <c r="B14">
         <v>953</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>242</v>
       </c>
       <c r="B15">
         <v>953</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>439</v>
+        <v>243</v>
       </c>
       <c r="B16">
         <v>940</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>439</v>
+        <v>129</v>
       </c>
       <c r="B17">
         <v>953</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>347</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>349</v>
@@ -3266,7 +3266,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>351</v>
@@ -3277,7 +3277,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>352</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>354</v>
@@ -3299,7 +3299,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>356</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>358</v>
@@ -3321,7 +3321,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>129</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>360</v>
@@ -3332,7 +3332,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>362</v>
@@ -3343,7 +3343,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
         <v>364</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>366</v>
@@ -3365,7 +3365,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>368</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="B14" t="s">
         <v>370</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="B15" t="s">
         <v>372</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
         <v>374</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
         <v>376</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>378</v>
@@ -3431,7 +3431,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
         <v>380</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
         <v>378</v>
@@ -3453,7 +3453,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
         <v>378</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="B22" t="s">
         <v>378</v>
@@ -3475,7 +3475,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
         <v>378</v>
@@ -3486,7 +3486,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
         <v>378</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
         <v>382</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
         <v>384</v>
@@ -3519,7 +3519,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="B27" t="s">
         <v>378</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="B28" t="s">
         <v>378</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="B29" t="s">
         <v>378</v>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="B30" t="s">
         <v>386</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
         <v>378</v>
@@ -3574,7 +3574,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="B32" t="s">
         <v>388</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
         <v>390</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
         <v>392</v>
@@ -3607,7 +3607,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>176</v>
       </c>
       <c r="B35" t="s">
         <v>378</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s">
         <v>378</v>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
         <v>394</v>
@@ -3640,7 +3640,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
         <v>396</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
         <v>398</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>192</v>
       </c>
       <c r="B40" t="s">
         <v>400</v>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>129</v>
+        <v>195</v>
       </c>
       <c r="B41" t="s">
         <v>402</v>
@@ -3684,7 +3684,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>129</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
         <v>404</v>
@@ -3695,7 +3695,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>129</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
         <v>406</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="B44" t="s">
         <v>378</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
         <v>408</v>
@@ -3728,7 +3728,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>434</v>
       </c>
       <c r="B46" t="s">
         <v>378</v>
@@ -4145,7 +4145,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
@@ -4174,272 +4174,122 @@
       <c r="B2" t="s">
         <v>268</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="G2" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>280</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>284</v>
-      </c>
-      <c r="G3" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" t="s">
-        <v>290</v>
-      </c>
-      <c r="I3" t="s">
-        <v>294</v>
-      </c>
-      <c r="J3" t="s">
-        <v>299</v>
-      </c>
-      <c r="K3" t="s">
-        <v>302</v>
-      </c>
-      <c r="L3" t="s">
-        <v>305</v>
-      </c>
-      <c r="M3" t="s">
-        <v>308</v>
-      </c>
-      <c r="N3" t="s">
-        <v>313</v>
-      </c>
-      <c r="O3" t="s">
-        <v>316</v>
-      </c>
-      <c r="P3" t="s">
-        <v>430</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>441</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="D4" t="s">
         <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>138</v>
+        <v>273</v>
       </c>
       <c r="F4" t="s">
         <v>138</v>
       </c>
       <c r="G4" t="s">
-        <v>442</v>
-      </c>
-      <c r="H4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>443</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" t="s">
-        <v>138</v>
-      </c>
-      <c r="L4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M4" t="s">
-        <v>138</v>
-      </c>
-      <c r="N4" t="s">
-        <v>138</v>
-      </c>
-      <c r="O4" t="s">
-        <v>138</v>
-      </c>
-      <c r="P4" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>440</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>446</v>
+        <v>324</v>
       </c>
       <c r="D5" t="s">
-        <v>447</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>325</v>
       </c>
       <c r="F5" t="s">
         <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" t="s">
-        <v>138</v>
-      </c>
-      <c r="I5" t="s">
-        <v>138</v>
-      </c>
-      <c r="J5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K5" t="s">
-        <v>138</v>
-      </c>
-      <c r="L5" t="s">
-        <v>138</v>
-      </c>
-      <c r="M5" t="s">
-        <v>138</v>
-      </c>
-      <c r="N5" t="s">
-        <v>138</v>
-      </c>
-      <c r="O5" t="s">
-        <v>138</v>
-      </c>
-      <c r="P5" t="s">
-        <v>448</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>444</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="B6" t="s">
         <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>278</v>
       </c>
       <c r="D6" t="s">
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>279</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>278</v>
       </c>
       <c r="G6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J6" t="s">
-        <v>138</v>
-      </c>
-      <c r="K6" t="s">
-        <v>138</v>
-      </c>
-      <c r="L6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M6" t="s">
-        <v>449</v>
-      </c>
-      <c r="N6" t="s">
-        <v>450</v>
-      </c>
-      <c r="O6" t="s">
-        <v>449</v>
-      </c>
-      <c r="P6" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>303</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="B7" t="s">
-        <v>452</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>453</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>454</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>455</v>
+        <v>282</v>
       </c>
       <c r="F7" t="s">
-        <v>456</v>
+        <v>283</v>
       </c>
       <c r="G7" t="s">
-        <v>457</v>
-      </c>
-      <c r="H7" t="s">
-        <v>453</v>
-      </c>
-      <c r="I7" t="s">
-        <v>458</v>
-      </c>
-      <c r="J7" t="s">
-        <v>459</v>
-      </c>
-      <c r="K7" t="s">
-        <v>460</v>
-      </c>
-      <c r="L7" t="s">
-        <v>138</v>
-      </c>
-      <c r="M7" t="s">
-        <v>461</v>
-      </c>
-      <c r="N7" t="s">
-        <v>454</v>
-      </c>
-      <c r="O7" t="s">
-        <v>462</v>
-      </c>
-      <c r="P7" t="s">
-        <v>455</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>451</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
         <v>138</v>
@@ -4448,46 +4298,246 @@
         <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>464</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>464</v>
+        <v>286</v>
       </c>
       <c r="F8" t="s">
         <v>138</v>
       </c>
       <c r="G8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" t="s">
-        <v>465</v>
-      </c>
-      <c r="I8" t="s">
-        <v>466</v>
-      </c>
-      <c r="J8" t="s">
-        <v>138</v>
-      </c>
-      <c r="K8" t="s">
-        <v>138</v>
-      </c>
-      <c r="L8" t="s">
-        <v>464</v>
-      </c>
-      <c r="M8" t="s">
-        <v>466</v>
-      </c>
-      <c r="N8" t="s">
-        <v>138</v>
-      </c>
-      <c r="O8" t="s">
-        <v>138</v>
-      </c>
-      <c r="P8" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>463</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" t="s">
+        <v>333</v>
+      </c>
+      <c r="F9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" t="s">
+        <v>292</v>
+      </c>
+      <c r="F10" t="s">
+        <v>293</v>
+      </c>
+      <c r="G10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" t="s">
+        <v>297</v>
+      </c>
+      <c r="F11" t="s">
+        <v>298</v>
+      </c>
+      <c r="G11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" t="s">
+        <v>307</v>
+      </c>
+      <c r="G14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
+        <v>310</v>
+      </c>
+      <c r="E15" t="s">
+        <v>311</v>
+      </c>
+      <c r="F15" t="s">
+        <v>312</v>
+      </c>
+      <c r="G15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>313</v>
+      </c>
+      <c r="B16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" t="s">
+        <v>315</v>
+      </c>
+      <c r="F16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>316</v>
+      </c>
+      <c r="B17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" t="s">
+        <v>318</v>
+      </c>
+      <c r="E17" t="s">
+        <v>319</v>
+      </c>
+      <c r="F17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>430</v>
+      </c>
+      <c r="B18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" t="s">
+        <v>432</v>
+      </c>
+      <c r="D18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" t="s">
+        <v>433</v>
+      </c>
+      <c r="F18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4547,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -4524,176 +4574,186 @@
       <c r="B2" t="s">
         <v>268</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G2" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>321</v>
+        <v>166</v>
       </c>
       <c r="C3" t="s">
-        <v>322</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
-        <v>326</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>330</v>
+        <v>161</v>
       </c>
       <c r="F3" t="s">
-        <v>334</v>
-      </c>
-      <c r="G3" t="s">
-        <v>339</v>
-      </c>
-      <c r="H3" t="s">
-        <v>430</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>321</v>
       </c>
       <c r="B4" t="s">
-        <v>441</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="D4" t="s">
         <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>442</v>
+        <v>273</v>
       </c>
       <c r="F4" t="s">
-        <v>443</v>
+        <v>138</v>
       </c>
       <c r="G4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" t="s">
-        <v>440</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>322</v>
       </c>
       <c r="B5" t="s">
-        <v>445</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
-        <v>446</v>
+        <v>324</v>
       </c>
       <c r="D5" t="s">
-        <v>447</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>325</v>
       </c>
       <c r="F5" t="s">
         <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" t="s">
-        <v>448</v>
-      </c>
-      <c r="I5" t="s">
-        <v>444</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>326</v>
       </c>
       <c r="B6" t="s">
         <v>138</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>423</v>
       </c>
       <c r="F6" t="s">
-        <v>449</v>
+        <v>424</v>
       </c>
       <c r="G6" t="s">
-        <v>467</v>
-      </c>
-      <c r="H6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" t="s">
-        <v>303</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>330</v>
       </c>
       <c r="B7" t="s">
-        <v>452</v>
+        <v>332</v>
       </c>
       <c r="C7" t="s">
-        <v>453</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>468</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>457</v>
+        <v>333</v>
       </c>
       <c r="F7" t="s">
-        <v>469</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
-        <v>470</v>
-      </c>
-      <c r="H7" t="s">
-        <v>455</v>
-      </c>
-      <c r="I7" t="s">
-        <v>451</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>334</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>426</v>
       </c>
       <c r="C8" t="s">
         <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>471</v>
+        <v>427</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>428</v>
       </c>
       <c r="F8" t="s">
-        <v>472</v>
+        <v>429</v>
       </c>
       <c r="G8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" t="s">
-        <v>138</v>
-      </c>
-      <c r="I8" t="s">
-        <v>463</v>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>339</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F9" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>430</v>
+      </c>
+      <c r="B10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" t="s">
+        <v>433</v>
+      </c>
+      <c r="F10" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" t="s">
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>